<commit_message>
logging successful entries, auto delete processed rows.
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u139547\PycharmProjects\PythonProject\robozinho\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295322C4-1B05-4E77-B350-AC13A9F76B32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD272B1-66FB-4147-9279-47FB9C9EE03E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4665" yWindow="2070" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -108,8 +108,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AC9D7CFD-E3AB-4F85-8FBC-3647CFC11B69}" name="Tabela1" displayName="Tabela1" ref="A1:B12" totalsRowShown="0">
-  <autoFilter ref="A1:B12" xr:uid="{AC9D7CFD-E3AB-4F85-8FBC-3647CFC11B69}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AC9D7CFD-E3AB-4F85-8FBC-3647CFC11B69}" name="Tabela1" displayName="Tabela1" ref="A1:B89" totalsRowShown="0">
+  <autoFilter ref="A1:B89" xr:uid="{AC9D7CFD-E3AB-4F85-8FBC-3647CFC11B69}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{4C00E28D-2F2E-4E3C-9E3B-6A602E9CF749}" name="Position"/>
     <tableColumn id="2" xr3:uid="{5E5863AA-1A8B-4755-9786-08FAE86D2617}" name="Planned Occupation Date" dataDxfId="0"/>
@@ -381,17 +381,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" customWidth="1"/>
     <col min="2" max="2" width="25.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -404,90 +403,706 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>627144</v>
+        <v>581965</v>
       </c>
       <c r="B2" s="1">
-        <v>45962</v>
+        <v>46006</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>532098</v>
+        <v>539795</v>
       </c>
       <c r="B3" s="1">
-        <v>45964</v>
+        <v>46113</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>580245</v>
+        <v>489408</v>
       </c>
       <c r="B4" s="1">
-        <v>45964</v>
+        <v>45978</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>10002157</v>
+        <v>570617</v>
       </c>
       <c r="B5" s="1">
-        <v>45962</v>
+        <v>45978</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>10004040</v>
+        <v>591484</v>
       </c>
       <c r="B6" s="1">
-        <v>45962</v>
+        <v>45992</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>10004096</v>
+        <v>492439</v>
       </c>
       <c r="B7" s="1">
-        <v>45962</v>
+        <v>45978</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>10004098</v>
+        <v>492486</v>
       </c>
       <c r="B8" s="1">
-        <v>45962</v>
+        <v>45978</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>598709</v>
+        <v>492447</v>
       </c>
       <c r="B9" s="1">
-        <v>45964</v>
+        <v>45978</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>511208</v>
+        <v>488873</v>
       </c>
       <c r="B10" s="1">
-        <v>45964</v>
+        <v>46054</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>489757</v>
+        <v>492620</v>
       </c>
       <c r="B11" s="1">
-        <v>45964</v>
+        <v>46054</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>513291</v>
+        <v>581829</v>
       </c>
       <c r="B12" s="1">
-        <v>45964</v>
+        <v>46054</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>578174</v>
+      </c>
+      <c r="B13" s="1">
+        <v>46006</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>581823</v>
+      </c>
+      <c r="B14" s="1">
+        <v>46006</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>577082</v>
+      </c>
+      <c r="B15" s="1">
+        <v>46054</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>578210</v>
+      </c>
+      <c r="B16" s="1">
+        <v>46006</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>489604</v>
+      </c>
+      <c r="B17" s="1">
+        <v>45978</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>601846</v>
+      </c>
+      <c r="B18" s="1">
+        <v>45978</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>437497</v>
+      </c>
+      <c r="B19" s="1">
+        <v>46006</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>601760</v>
+      </c>
+      <c r="B20" s="1">
+        <v>45978</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>512661</v>
+      </c>
+      <c r="B21" s="1">
+        <v>45978</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>578257</v>
+      </c>
+      <c r="B22" s="1">
+        <v>45978</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>489637</v>
+      </c>
+      <c r="B23" s="1">
+        <v>45978</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>489734</v>
+      </c>
+      <c r="B24" s="1">
+        <v>45978</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>499165</v>
+      </c>
+      <c r="B25" s="1">
+        <v>45978</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>601659</v>
+      </c>
+      <c r="B26" s="1">
+        <v>45978</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>582046</v>
+      </c>
+      <c r="B27" s="1">
+        <v>45978</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>10005085</v>
+      </c>
+      <c r="B28" s="1">
+        <v>46054</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>10005140</v>
+      </c>
+      <c r="B29" s="1">
+        <v>46054</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>591498</v>
+      </c>
+      <c r="B30" s="1">
+        <v>45992</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>492000</v>
+      </c>
+      <c r="B31" s="1">
+        <v>46054</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>570871</v>
+      </c>
+      <c r="B32" s="1">
+        <v>45978</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>575042</v>
+      </c>
+      <c r="B33" s="1">
+        <v>46006</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>10000412</v>
+      </c>
+      <c r="B34" s="1">
+        <v>46006</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>570732</v>
+      </c>
+      <c r="B35" s="1">
+        <v>46006</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>614693</v>
+      </c>
+      <c r="B36" s="1">
+        <v>45978</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>10001730</v>
+      </c>
+      <c r="B37" s="1">
+        <v>45978</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>10001731</v>
+      </c>
+      <c r="B38" s="1">
+        <v>45978</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>570758</v>
+      </c>
+      <c r="B39" s="1">
+        <v>46006</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>10006526</v>
+      </c>
+      <c r="B40" s="1">
+        <v>46006</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>10006512</v>
+      </c>
+      <c r="B41" s="1">
+        <v>46054</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>10006513</v>
+      </c>
+      <c r="B42" s="1">
+        <v>46054</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>559904</v>
+      </c>
+      <c r="B43" s="1">
+        <v>46006</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>10002729</v>
+      </c>
+      <c r="B44" s="1">
+        <v>46006</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>10006519</v>
+      </c>
+      <c r="B45" s="1">
+        <v>46006</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>10006522</v>
+      </c>
+      <c r="B46" s="1">
+        <v>46006</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>570785</v>
+      </c>
+      <c r="B47" s="1">
+        <v>46006</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>10005108</v>
+      </c>
+      <c r="B48" s="1">
+        <v>46006</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>10005444</v>
+      </c>
+      <c r="B49" s="1">
+        <v>46006</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>578127</v>
+      </c>
+      <c r="B50" s="1">
+        <v>46006</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>10005112</v>
+      </c>
+      <c r="B51" s="1">
+        <v>46006</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>600922</v>
+      </c>
+      <c r="B52" s="1">
+        <v>46054</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>578138</v>
+      </c>
+      <c r="B53" s="1">
+        <v>46054</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>570935</v>
+      </c>
+      <c r="B54" s="1">
+        <v>45978</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>570796</v>
+      </c>
+      <c r="B55" s="1">
+        <v>46006</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>614621</v>
+      </c>
+      <c r="B56" s="1">
+        <v>45978</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>488891</v>
+      </c>
+      <c r="B57" s="1">
+        <v>46054</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>578156</v>
+      </c>
+      <c r="B58" s="1">
+        <v>46054</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>489390</v>
+      </c>
+      <c r="B59" s="1">
+        <v>45992</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>491877</v>
+      </c>
+      <c r="B60" s="1">
+        <v>45978</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>581993</v>
+      </c>
+      <c r="B61" s="1">
+        <v>46006</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>570711</v>
+      </c>
+      <c r="B62" s="1">
+        <v>46006</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>570714</v>
+      </c>
+      <c r="B63" s="1">
+        <v>46006</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>491887</v>
+      </c>
+      <c r="B64" s="1">
+        <v>46006</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>10005026</v>
+      </c>
+      <c r="B65" s="1">
+        <v>46006</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>488879</v>
+      </c>
+      <c r="B66" s="1">
+        <v>46054</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>492291</v>
+      </c>
+      <c r="B67" s="1">
+        <v>45992</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>601612</v>
+      </c>
+      <c r="B68" s="1">
+        <v>46054</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>591493</v>
+      </c>
+      <c r="B69" s="1">
+        <v>45992</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>581926</v>
+      </c>
+      <c r="B70" s="1">
+        <v>46054</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>10000687</v>
+      </c>
+      <c r="B71" s="1">
+        <v>46054</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>513251</v>
+      </c>
+      <c r="B72" s="1">
+        <v>45992</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>503436</v>
+      </c>
+      <c r="B73" s="1">
+        <v>46054</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>600911</v>
+      </c>
+      <c r="B74" s="1">
+        <v>46054</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>541282</v>
+      </c>
+      <c r="B75" s="1">
+        <v>46054</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>498934</v>
+      </c>
+      <c r="B76" s="1">
+        <v>46054</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>601615</v>
+      </c>
+      <c r="B77" s="1">
+        <v>46054</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>10000694</v>
+      </c>
+      <c r="B78" s="1">
+        <v>46054</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>540404</v>
+      </c>
+      <c r="B79" s="1">
+        <v>46054</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>10005778</v>
+      </c>
+      <c r="B80" s="1">
+        <v>45992</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>10006495</v>
+      </c>
+      <c r="B81" s="1">
+        <v>45978</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>10006499</v>
+      </c>
+      <c r="B82" s="1">
+        <v>45978</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>10006516</v>
+      </c>
+      <c r="B83" s="1">
+        <v>46054</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>10006517</v>
+      </c>
+      <c r="B84" s="1">
+        <v>46006</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>10006518</v>
+      </c>
+      <c r="B85" s="1">
+        <v>46006</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>581776</v>
+      </c>
+      <c r="B86" s="1">
+        <v>45999</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>581913</v>
+      </c>
+      <c r="B87" s="1">
+        <v>45999</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>488891</v>
+      </c>
+      <c r="B88" s="1">
+        <v>45999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>498934</v>
+      </c>
+      <c r="B89" s="1">
+        <v>45999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>